<commit_message>
GET list reject participants & Fix bugs of GET Event by id
</commit_message>
<xml_diff>
--- a/resources/participants.xlsx
+++ b/resources/participants.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trongbui/Projects.NET/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFEDE717-866E-443B-A351-D7436AE0D3B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA7D1D88-2196-AB46-B618-F2C62FD5C82D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1440" yWindow="1900" windowWidth="24600" windowHeight="14160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sample" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="58">
   <si>
     <t>Personal ID</t>
   </si>
@@ -185,6 +185,15 @@
   </si>
   <si>
     <t>09080989080</t>
+  </si>
+  <si>
+    <t>23/03/2022</t>
+  </si>
+  <si>
+    <t>25/03/2022</t>
+  </si>
+  <si>
+    <t>30/03/2022</t>
   </si>
 </sst>
 </file>
@@ -195,7 +204,7 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -564,16 +573,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="10" width="30.84375" customWidth="1"/>
+    <col min="1" max="10" width="30.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -605,7 +614,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>36</v>
       </c>
@@ -627,8 +636,8 @@
       <c r="G2" t="s">
         <v>13</v>
       </c>
-      <c r="H2" t="s">
-        <v>14</v>
+      <c r="H2" s="1" t="s">
+        <v>55</v>
       </c>
       <c r="I2" t="s">
         <v>15</v>
@@ -637,7 +646,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>37</v>
       </c>
@@ -659,7 +668,7 @@
       <c r="G3" t="s">
         <v>18</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="1" t="s">
         <v>14</v>
       </c>
       <c r="I3" t="s">
@@ -669,7 +678,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>38</v>
       </c>
@@ -691,8 +700,8 @@
       <c r="G4" t="s">
         <v>22</v>
       </c>
-      <c r="H4" t="s">
-        <v>14</v>
+      <c r="H4" s="1" t="s">
+        <v>56</v>
       </c>
       <c r="I4" t="s">
         <v>23</v>
@@ -701,7 +710,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>39</v>
       </c>
@@ -723,7 +732,7 @@
       <c r="G5" t="s">
         <v>26</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="1" t="s">
         <v>14</v>
       </c>
       <c r="I5" t="s">
@@ -733,7 +742,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>40</v>
       </c>
@@ -755,8 +764,8 @@
       <c r="G6" t="s">
         <v>30</v>
       </c>
-      <c r="H6" t="s">
-        <v>14</v>
+      <c r="H6" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="I6" t="s">
         <v>31</v>
@@ -765,7 +774,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>41</v>
       </c>
@@ -787,7 +796,7 @@
       <c r="G7" t="s">
         <v>34</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" s="1" t="s">
         <v>14</v>
       </c>
       <c r="I7" t="s">
@@ -801,7 +810,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:G1 C7:E7 D2:G2 E3:G3 D4:G4 C5:E5 C6:E6 J5 H1:J1 H7:J7 H2:J2 H3:J3 H4:J4 H5 H6:J6 G7 G5 G6" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:G1 C7:E7 D2:G2 E3:G3 D4:G4 C5:E5 C6:E6 J5 H1:J1 H7:J7 I2:J2 H3:J3 I4:J4 H5 I6:J6 G7 G5 G6" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
API GET general information of Dashboard
</commit_message>
<xml_diff>
--- a/resources/participants.xlsx
+++ b/resources/participants.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trongbui/Projects.NET/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBE780DA-5EC1-994E-8B1F-D5F92C131CDA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1D42F0B-B5BF-8742-A858-A3A9766D959E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1440" yWindow="1900" windowWidth="24600" windowHeight="14160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="97">
   <si>
     <t>Personal ID</t>
   </si>
@@ -214,9 +214,6 @@
     <t>cvl@gmail.com</t>
   </si>
   <si>
-    <t>11/12/2021</t>
-  </si>
-  <si>
     <t>B Negative</t>
   </si>
   <si>
@@ -238,9 +235,6 @@
     <t>tvh@gmail.com</t>
   </si>
   <si>
-    <t>12/12/2021</t>
-  </si>
-  <si>
     <t>A Negative</t>
   </si>
   <si>
@@ -280,9 +274,6 @@
     <t>ltt@gmail.com</t>
   </si>
   <si>
-    <t>10/12/2021</t>
-  </si>
-  <si>
     <t>O Negative</t>
   </si>
   <si>
@@ -305,6 +296,21 @@
   </si>
   <si>
     <t>AB Positive</t>
+  </si>
+  <si>
+    <t>03/04/2022</t>
+  </si>
+  <si>
+    <t>01/04/2022</t>
+  </si>
+  <si>
+    <t>02/04/2022</t>
+  </si>
+  <si>
+    <t>04/04/2022</t>
+  </si>
+  <si>
+    <t>01/04/2021</t>
   </si>
 </sst>
 </file>
@@ -696,8 +702,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -952,10 +958,10 @@
         <v>63</v>
       </c>
       <c r="H8" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="I8" t="s">
         <v>64</v>
-      </c>
-      <c r="I8" t="s">
-        <v>65</v>
       </c>
       <c r="J8">
         <v>200</v>
@@ -963,31 +969,31 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B9" t="s">
         <v>66</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>68</v>
       </c>
       <c r="D9" t="s">
         <v>28</v>
       </c>
       <c r="E9" t="s">
+        <v>68</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="G9" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="H9" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="I9" t="s">
         <v>71</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="I9" t="s">
-        <v>73</v>
       </c>
       <c r="J9">
         <v>178</v>
@@ -995,28 +1001,28 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B10" t="s">
+        <v>73</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="B10" t="s">
-        <v>75</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>76</v>
       </c>
       <c r="D10" t="s">
         <v>10</v>
       </c>
       <c r="E10" t="s">
+        <v>75</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G10" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>79</v>
-      </c>
       <c r="H10" s="1" t="s">
-        <v>72</v>
+        <v>94</v>
       </c>
       <c r="I10" t="s">
         <v>31</v>
@@ -1027,31 +1033,31 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B11" t="s">
+        <v>79</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="B11" t="s">
-        <v>81</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>82</v>
       </c>
       <c r="D11" t="s">
         <v>28</v>
       </c>
       <c r="E11" t="s">
+        <v>81</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G11" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="H11" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="I11" t="s">
         <v>84</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="I11" t="s">
-        <v>87</v>
       </c>
       <c r="J11">
         <v>199</v>
@@ -1059,31 +1065,31 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B12" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D12" t="s">
         <v>10</v>
       </c>
       <c r="E12" t="s">
+        <v>88</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="I12" t="s">
         <v>91</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="I12" t="s">
-        <v>94</v>
       </c>
       <c r="J12">
         <v>144</v>

</xml_diff>

<commit_message>
Add Default Data from JSON file
</commit_message>
<xml_diff>
--- a/resources/participants.xlsx
+++ b/resources/participants.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trongbui/Projects.NET/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1D42F0B-B5BF-8742-A858-A3A9766D959E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7E2E44F-15A5-AD47-A80F-6F70D336F324}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1440" yWindow="1900" windowWidth="24600" windowHeight="14160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -67,9 +67,6 @@
     <t>28/03/2022</t>
   </si>
   <si>
-    <t>A Positive</t>
-  </si>
-  <si>
     <t>Hau Giang</t>
   </si>
   <si>
@@ -79,9 +76,6 @@
     <t>lvd@gmail.com</t>
   </si>
   <si>
-    <t>Rh Negative</t>
-  </si>
-  <si>
     <t>An Giang</t>
   </si>
   <si>
@@ -91,9 +85,6 @@
     <t>nnt@gmail.com</t>
   </si>
   <si>
-    <t>Rh Positive</t>
-  </si>
-  <si>
     <t>11/04/1985</t>
   </si>
   <si>
@@ -115,9 +106,6 @@
     <t>coolboy@gmail.com</t>
   </si>
   <si>
-    <t>B Positive</t>
-  </si>
-  <si>
     <t>30/04/2004</t>
   </si>
   <si>
@@ -127,9 +115,6 @@
     <t>soinhoyeuem@gmail.com</t>
   </si>
   <si>
-    <t>AB Negative</t>
-  </si>
-  <si>
     <t>000011112222</t>
   </si>
   <si>
@@ -175,9 +160,6 @@
     <t>Nguyễn Tất Thành</t>
   </si>
   <si>
-    <t>O Positive</t>
-  </si>
-  <si>
     <t>0909090898</t>
   </si>
   <si>
@@ -214,9 +196,6 @@
     <t>cvl@gmail.com</t>
   </si>
   <si>
-    <t>B Negative</t>
-  </si>
-  <si>
     <t>234561234567</t>
   </si>
   <si>
@@ -235,9 +214,6 @@
     <t>tvh@gmail.com</t>
   </si>
   <si>
-    <t>A Negative</t>
-  </si>
-  <si>
     <t>542148129410</t>
   </si>
   <si>
@@ -274,9 +250,6 @@
     <t>ltt@gmail.com</t>
   </si>
   <si>
-    <t>O Negative</t>
-  </si>
-  <si>
     <t>749218841941</t>
   </si>
   <si>
@@ -295,9 +268,6 @@
     <t>nguyentrai@gmail.com</t>
   </si>
   <si>
-    <t>AB Positive</t>
-  </si>
-  <si>
     <t>03/04/2022</t>
   </si>
   <si>
@@ -311,6 +281,36 @@
   </si>
   <si>
     <t>01/04/2021</t>
+  </si>
+  <si>
+    <t>A positive</t>
+  </si>
+  <si>
+    <t>Rh negative</t>
+  </si>
+  <si>
+    <t>Rh positive</t>
+  </si>
+  <si>
+    <t>O positive</t>
+  </si>
+  <si>
+    <t>B positive</t>
+  </si>
+  <si>
+    <t>AB negative</t>
+  </si>
+  <si>
+    <t>B negative</t>
+  </si>
+  <si>
+    <t>A negative</t>
+  </si>
+  <si>
+    <t>O negative</t>
+  </si>
+  <si>
+    <t>AB positive</t>
   </si>
 </sst>
 </file>
@@ -702,8 +702,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -745,13 +745,13 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D2" t="s">
         <v>10</v>
@@ -766,10 +766,10 @@
         <v>13</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="I2" t="s">
-        <v>15</v>
+        <v>87</v>
       </c>
       <c r="J2">
         <v>125</v>
@@ -777,31 +777,31 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B3" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="D3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>14</v>
       </c>
       <c r="I3" t="s">
-        <v>19</v>
+        <v>88</v>
       </c>
       <c r="J3">
         <v>150</v>
@@ -809,31 +809,31 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D4" t="s">
         <v>10</v>
       </c>
       <c r="E4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="H4" s="1" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="I4" t="s">
-        <v>23</v>
+        <v>89</v>
       </c>
       <c r="J4">
         <v>243</v>
@@ -841,31 +841,31 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B5" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D5" t="s">
         <v>10</v>
       </c>
       <c r="E5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>14</v>
       </c>
       <c r="I5" t="s">
-        <v>51</v>
+        <v>90</v>
       </c>
       <c r="J5">
         <v>125</v>
@@ -873,31 +873,31 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" t="s">
-        <v>29</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="H6" s="1" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="I6" t="s">
-        <v>31</v>
+        <v>91</v>
       </c>
       <c r="J6">
         <v>100</v>
@@ -905,31 +905,31 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B7" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D7" t="s">
         <v>10</v>
       </c>
       <c r="E7" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>14</v>
       </c>
       <c r="I7" t="s">
-        <v>35</v>
+        <v>92</v>
       </c>
       <c r="J7">
         <v>100</v>
@@ -937,31 +937,31 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B8" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="D8" t="s">
         <v>10</v>
       </c>
       <c r="E8" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="H8" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="I8" t="s">
         <v>93</v>
-      </c>
-      <c r="I8" t="s">
-        <v>64</v>
       </c>
       <c r="J8">
         <v>200</v>
@@ -969,31 +969,31 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="B9" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="D9" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E9" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="I9" t="s">
-        <v>71</v>
+        <v>94</v>
       </c>
       <c r="J9">
         <v>178</v>
@@ -1001,31 +1001,31 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="B10" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="D10" t="s">
         <v>10</v>
       </c>
       <c r="E10" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="I10" t="s">
-        <v>31</v>
+        <v>91</v>
       </c>
       <c r="J10">
         <v>163</v>
@@ -1033,31 +1033,31 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="B11" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="D11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E11" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="H11" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="I11" t="s">
         <v>95</v>
-      </c>
-      <c r="I11" t="s">
-        <v>84</v>
       </c>
       <c r="J11">
         <v>199</v>
@@ -1065,31 +1065,31 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="B12" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="D12" t="s">
         <v>10</v>
       </c>
       <c r="E12" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="H12" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="I12" t="s">
         <v>96</v>
-      </c>
-      <c r="I12" t="s">
-        <v>91</v>
       </c>
       <c r="J12">
         <v>144</v>
@@ -1137,7 +1137,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId6"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:G1 C7:E7 D2:G2 E3:G3 D4:G4 C5:E5 C6:E6 J5 H1:J1 H7:J7 I2:J2 H3:J3 I4:J4 H5 I6:J6 G7 G5 G6" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:G1 C7:E7 D2:G2 E3:G3 D4:G4 C5:E5 C6:E6 J5 H1:J1 H7 J2 H3 J4 H5 J6 G7 G5 G6 J3 J7" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>